<commit_message>
Updated Lino Salinas hours for L/A renewal
</commit_message>
<xml_diff>
--- a/Data/La_hr_lsalinas_start_y17_pp22.xlsx
+++ b/Data/La_hr_lsalinas_start_y17_pp22.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles.Burks\MyGit\La_tracker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99F35960-1A35-4E88-BDFF-C3929760C5E5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ACF5A1A0-262A-4376-BE3D-33F5FAE72546}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16932" windowHeight="8244" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16932" windowHeight="8244" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataform" sheetId="1" r:id="rId1"/>
     <sheet name="Grid" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Dataform!$A$1:$S$33</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>Year</t>
   </si>
@@ -113,6 +116,9 @@
   </si>
   <si>
     <t>Difference:</t>
+  </si>
+  <si>
+    <t>Days</t>
   </si>
 </sst>
 </file>
@@ -453,11 +459,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S32"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3:S21"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1475,7 +1481,34 @@
       </c>
       <c r="E22" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>72</v>
+      </c>
+      <c r="G22">
+        <v>8</v>
+      </c>
+      <c r="H22">
+        <v>8</v>
+      </c>
+      <c r="I22">
+        <v>8</v>
+      </c>
+      <c r="J22">
+        <v>8</v>
+      </c>
+      <c r="K22">
+        <v>8</v>
+      </c>
+      <c r="N22">
+        <v>8</v>
+      </c>
+      <c r="O22">
+        <v>8</v>
+      </c>
+      <c r="P22">
+        <v>8</v>
+      </c>
+      <c r="Q22">
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
@@ -1604,7 +1637,7 @@
       </c>
       <c r="E30">
         <f>SUM(E3:E28)</f>
-        <v>1308</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -1621,7 +1654,16 @@
       </c>
       <c r="E32">
         <f>E31-E30</f>
-        <v>-269</v>
+        <v>-341</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33">
+        <f>COUNT(F3:S28)</f>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1638,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2415,6 +2457,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Excel and csv hours reports
</commit_message>
<xml_diff>
--- a/Data/La_hr_lsalinas_start_y17_pp22.xlsx
+++ b/Data/La_hr_lsalinas_start_y17_pp22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles.Burks\MyGit\La_tracker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ACF5A1A0-262A-4376-BE3D-33F5FAE72546}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F5F92BAB-5710-43BD-991A-A8D2C40021BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16932" windowHeight="8244" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16932" windowHeight="8244" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataform" sheetId="1" r:id="rId1"/>
@@ -461,9 +461,9 @@
   </sheetPr>
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22:R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1680,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2406,6 +2406,33 @@
       <c r="B21">
         <v>15</v>
       </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>8</v>
+      </c>
+      <c r="G21">
+        <v>8</v>
+      </c>
+      <c r="H21">
+        <v>8</v>
+      </c>
+      <c r="K21">
+        <v>8</v>
+      </c>
+      <c r="L21">
+        <v>8</v>
+      </c>
+      <c r="M21">
+        <v>8</v>
+      </c>
+      <c r="N21">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1">

</xml_diff>